<commit_message>
PROS-14717 LionJP Adjacency KPI
</commit_message>
<xml_diff>
--- a/Projects/LIONJP_SAND/Data/setup.xlsx
+++ b/Projects/LIONJP_SAND/Data/setup.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">ADJACENCY</t>
   </si>
   <si>
-    <t xml:space="preserve">PRODUCT_GROUP_ADJACENCY_IN_WHOLE_STORE</t>
+    <t xml:space="preserve">ADJACENCY_PRODUCT_GROUP_IN_SCENE_TYPE</t>
   </si>
   <si>
     <t xml:space="preserve">FSOS</t>
@@ -147,14 +147,14 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.4336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>